<commit_message>
CARLA-3 Priliminary Darft of DPEs and DD. DD has a lot of missings because there are lot of questions to be asked.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89812AA1-E44D-43B2-A662-AA42658104EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F382ADD-167B-4EF1-BD0A-D97CBD77D224}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="204">
   <si>
     <t>index</t>
   </si>
@@ -578,41 +578,6 @@
   </si>
   <si>
     <t>f2_diabetes_year</t>
-  </si>
-  <si>
-    <r>
-      <t>f1_diabetes_year-format(as.Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(d_birth, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>format="%d/%m/%Y"),"%Y"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>f2_cancer1_inc</t>
@@ -701,12 +666,15 @@
   <si>
     <t>birth_place</t>
   </si>
+  <si>
+    <t>f1_diabetes_year-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,13 +729,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -798,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -875,16 +836,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1229,23 +1180,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H15" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1280,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
@@ -1306,7 +1257,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1283,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1309,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
@@ -1375,7 +1326,7 @@
         <v>148</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>136</v>
@@ -1384,7 +1335,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1410,7 +1361,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1387,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="25" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>25</v>
       </c>
@@ -1453,7 +1404,7 @@
         <v>142</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>136</v>
@@ -1462,7 +1413,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1473,11 +1424,9 @@
         <v>13</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>142</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="G9" s="7"/>
       <c r="J9" s="8" t="s">
         <v>151</v>
       </c>
@@ -1485,7 +1434,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1457,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -1534,7 +1483,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1545,16 +1494,16 @@
         <v>18</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>145</v>
       </c>
       <c r="H12" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>151</v>
@@ -1563,7 +1512,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1589,7 +1538,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -1615,33 +1564,30 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="29" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="30" t="s">
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="H15" s="29">
-        <v>1</v>
-      </c>
-      <c r="J15" s="32" t="s">
+      <c r="J15" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>41</v>
       </c>
@@ -1658,7 +1604,7 @@
         <v>148</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>136</v>
@@ -1667,7 +1613,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1690,7 +1636,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -1716,7 +1662,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1739,7 +1685,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
@@ -1765,33 +1711,33 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="2:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+    <row r="21" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="G21" s="31" t="s">
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="J21" s="32" t="s">
+      <c r="J21" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="K21" s="32" t="s">
+      <c r="K21" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>53</v>
       </c>
@@ -1818,7 +1764,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -1844,7 +1790,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
         <v>57</v>
       </c>
@@ -1855,7 +1801,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G24" t="s">
         <v>148</v>
@@ -1870,7 +1816,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -1896,7 +1842,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>61</v>
       </c>
@@ -1922,7 +1868,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>63</v>
       </c>
@@ -1945,7 +1891,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -1968,7 +1914,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -1991,7 +1937,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -2014,7 +1960,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>71</v>
       </c>
@@ -2037,7 +1983,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -2060,7 +2006,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>75</v>
       </c>
@@ -2083,7 +2029,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
         <v>77</v>
       </c>
@@ -2106,7 +2052,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
         <v>79</v>
       </c>
@@ -2129,7 +2075,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>81</v>
       </c>
@@ -2152,7 +2098,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>83</v>
       </c>
@@ -2175,7 +2121,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="2:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
         <v>85</v>
       </c>
@@ -2185,10 +2131,10 @@
       <c r="D38" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="H38" s="33" t="s">
+      <c r="G38" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="H38" s="29" t="s">
         <v>153</v>
       </c>
       <c r="J38" s="12" t="s">
@@ -2198,7 +2144,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>87</v>
       </c>
@@ -2221,7 +2167,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>89</v>
       </c>
@@ -2247,7 +2193,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>91</v>
       </c>
@@ -2258,7 +2204,7 @@
         <v>18</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>145</v>
@@ -2273,7 +2219,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="2:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>93</v>
       </c>
@@ -2299,7 +2245,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2326,7 +2272,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>97</v>
       </c>
@@ -2349,7 +2295,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -2372,7 +2318,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>101</v>
       </c>
@@ -2395,7 +2341,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>103</v>
       </c>
@@ -2418,7 +2364,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>105</v>
       </c>
@@ -2442,7 +2388,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="30" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>107</v>
       </c>
@@ -2471,7 +2417,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>109</v>
       </c>
@@ -2500,7 +2446,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="30" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>111</v>
       </c>
@@ -2529,7 +2475,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>113</v>
       </c>
@@ -2556,36 +2502,36 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="30" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
+    <row r="53" spans="2:11" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="23" t="s">
+      <c r="F53" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I53" s="24" t="s">
+      <c r="H53" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I53" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="J53" s="15" t="s">
+      <c r="J53" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="K53" s="15" t="s">
+      <c r="K53" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>117</v>
       </c>
@@ -2596,13 +2542,13 @@
         <v>13</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>148</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4" t="s">
@@ -2612,22 +2558,19 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
+    <row r="55" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
+        <v>188</v>
+      </c>
       <c r="J55" s="2" t="s">
         <v>151</v>
       </c>
@@ -2635,7 +2578,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="30" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -2646,13 +2589,13 @@
         <v>18</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>145</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I56" s="24" t="s">
         <v>179</v>
@@ -2664,7 +2607,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>124</v>
       </c>
@@ -2675,7 +2618,7 @@
         <v>13</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>139</v>
@@ -2691,24 +2634,22 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
+    <row r="58" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
       <c r="J58" s="8" t="s">
         <v>151</v>
       </c>
@@ -2716,7 +2657,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>128</v>
       </c>
@@ -2740,7 +2681,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>130</v>
       </c>
@@ -2764,7 +2705,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
CARLA-3 I have now carefully gone through all the DPEs and DD. Priliminary documents looks fine except errors in the ff variable Edu(I need help with coding) The rest of the errors in the variables need further answers for proper coding(eg. Age related variables for calculation)
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F382ADD-167B-4EF1-BD0A-D97CBD77D224}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1040E7-9405-4BE1-B48E-633EDCFD0F62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="198">
   <si>
     <t>index</t>
   </si>
@@ -385,9 +385,6 @@
     <t>Type of Cancer (ICD 10, 3 digits,e.g. C18.3)</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>AGE_CANCER</t>
   </si>
   <si>
@@ -424,9 +421,6 @@
     <t>Age at end of follow-up [years]</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>id_creation</t>
   </si>
   <si>
@@ -445,9 +439,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>school</t>
-  </si>
-  <si>
     <t>case_when</t>
   </si>
   <si>
@@ -496,9 +487,6 @@
     <t>vit_min</t>
   </si>
   <si>
-    <t>Period_current; Ovariectomy</t>
-  </si>
-  <si>
     <t>proximate</t>
   </si>
   <si>
@@ -535,30 +523,15 @@
     <t>fam_cancer</t>
   </si>
   <si>
-    <t>f1_mi_i_inc;   f2_mi_i_inc</t>
-  </si>
-  <si>
     <t>recode (1= 1; 2 = 0;)</t>
   </si>
   <si>
-    <t>f1_mi_1_year-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f1_stroke_i_inc; f2_stoke_i_inc; </t>
-  </si>
-  <si>
     <t>f1_stroke_first_year_inc</t>
   </si>
   <si>
     <t>f1_stroke_first_year_inc-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
   </si>
   <si>
-    <t>f1_hyp2</t>
-  </si>
-  <si>
-    <t>f1_hyp2-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
-  </si>
-  <si>
     <t>date of diagnose and the date of birth</t>
   </si>
   <si>
@@ -568,16 +541,7 @@
     <t>measured HF via echocardiography, symptoms and pBNP at FU1</t>
   </si>
   <si>
-    <t>f1_age; f2_insuff</t>
-  </si>
-  <si>
     <t>f1_age-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
-  </si>
-  <si>
-    <t>f2_diabetes2</t>
-  </si>
-  <si>
-    <t>f2_diabetes_year</t>
   </si>
   <si>
     <t>f2_cancer1_inc</t>
@@ -651,23 +615,53 @@
     <t>recode(1= 1; 2 = 0; 9=0;)</t>
   </si>
   <si>
-    <t xml:space="preserve">f1_mi_1_year; </t>
-  </si>
-  <si>
-    <t>recode(1= 0; 2 = 1; 3=5;4=6;5=7;6=7;7=9;)</t>
+    <t>birth_place</t>
   </si>
   <si>
     <t>case_when(
-work_status == 1 ~ 0; work_status == 2~ 1;work_status == 3~ 5;work_status == 4 ~ 6;
-work_status== 5 | work_status == 6 ~ 7;
-work_status == 7 ~ 9;
-employ== 1 ~ 1; employ == 2 ~ 2; employ == 3 ~ 2 ; employ== 4 ~ 7 ;</t>
-  </si>
-  <si>
-    <t>birth_place</t>
-  </si>
-  <si>
-    <t>f1_diabetes_year-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
+work_status == 1 ~ 0,                                                                                                    work_status == 2~ 1,                                                                                                       work_status == 3~ 5,                                                                                                             work_status == 4 ~ 6;
+work_status== 5 | work_status == 6 ~ 7,
+work_status == 7 ~ 9,
+employ== 1 ~ 1,                                                                                                                            employ == 2 ~ 2,                                                                                                                              employ == 3 ~ 2,                                                                                                                    employ== 4 ~ 7, TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>School; occup_edu;          occup_edu_2;   occup_edu_h;             educ; educ3</t>
+  </si>
+  <si>
+    <t>"case_when(
+ School  %in% c(1) | occup_edu %in% c(1)| occup_edu_2 %in% c(1)| occup_edu_h%in% c(1)| educ %in% c(1)| educ3%in% c(1)~ 1L,                                       
+School  %in% c(2) | occup_edu %in% c(2)| occup_edu_2 %in% c(2)| occup_edu_h%in% c(2)| educ %in% c(2)| educ3%in% c(2)~ 2L,                            School %in% c(3,4) |  occup_edu  %in% c(3)| occup_edu_2%in% c(3)| occup_edu_h%in% c(3)| educ %in% c(3)| educ3%in% c(3)~ 3L,           
+School %in% c(5,6) | occup_edu %in% c(4)| occup_edu_2 %in% c(4)| occup_edu_h%in% c(4)| educ %in% c(4)~ 3L,                                                                School %in% c(5,6) | occup_edu%in% c(5)| occup_edu_2  %in% c(5)| occup_edu_h%in% c(5)| edu %in% c(5)~ 5L,                                                                     School%in% c(5,6) | occup_edu %in% c(6)| occup_edu_2  %in% c(6)| occup_edu_h%in% c(6)| educ%in% c(6)~ 6L,                                                                                     School %in% c(5,6) | occup_edu%in% c(7)| occup_edu_2  %in% c(7)| occup_edu_h%in% c(7)| educ %in% c(7)~ 7L,                                                                    School  %in% c(7) | occup_edu%in% c(8)| occup_edu_2  %in% c(8)| occup_edu_h%in% c(8)~ 9L,                                                                                                         TRUE ~ NA_integer_)"</t>
+  </si>
+  <si>
+    <t>df &lt;- data.frame(
+  birth = c(
+    "A) foreigner",
+    "B) born in Germany, parents not from Germany or Poland",
+    "Some other category",
+    "D) emigrant from former USSR"
+  )
+)
+df &lt;- categorize_immigration_background(df)
+print(df)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f2_mi_i_inc</t>
+  </si>
+  <si>
+    <t>f2_mi_year</t>
+  </si>
+  <si>
+    <t>f2_mi_year-format(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
+  </si>
+  <si>
+    <t>f2_stoke_i_inc</t>
+  </si>
+  <si>
+    <t>f1_age</t>
+  </si>
+  <si>
+    <t>tod_dat -(as.Date(d_birth, format="%d/%m/%Y"),"%Y")</t>
   </si>
 </sst>
 </file>
@@ -828,17 +822,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1180,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B58" sqref="A58:XFD58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,30 +1225,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="26" t="s">
+      <c r="D2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="K2" s="25" t="s">
         <v>135</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,19 +1262,19 @@
         <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1294,45 +1288,45 @@
         <v>18</v>
       </c>
       <c r="F4" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="25" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>140</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1346,19 +1340,19 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1372,22 +1366,22 @@
         <v>13</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="25" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="25" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>25</v>
       </c>
@@ -1398,22 +1392,22 @@
         <v>13</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1424,14 +1418,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="G9" s="7"/>
+        <v>187</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>191</v>
+      </c>
       <c r="J9" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1445,16 +1444,16 @@
         <v>18</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1468,19 +1467,19 @@
         <v>18</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1494,22 +1493,22 @@
         <v>18</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1523,19 +1522,19 @@
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1549,22 +1548,22 @@
         <v>13</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1574,17 +1573,18 @@
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>158</v>
-      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>142</v>
+        <v>150</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1598,19 +1598,19 @@
         <v>13</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1624,16 +1624,16 @@
         <v>13</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1647,19 +1647,19 @@
         <v>13</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1673,16 +1673,16 @@
         <v>18</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1696,19 +1696,19 @@
         <v>13</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1722,19 +1722,19 @@
         <v>13</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="G21" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="K21" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1748,20 +1748,20 @@
         <v>13</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1775,19 +1775,19 @@
         <v>13</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1801,19 +1801,19 @@
         <v>13</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1827,19 +1827,19 @@
         <v>13</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G25" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1853,19 +1853,19 @@
         <v>13</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1879,16 +1879,16 @@
         <v>13</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1902,16 +1902,16 @@
         <v>13</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1925,16 +1925,16 @@
         <v>13</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1948,16 +1948,16 @@
         <v>13</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1971,16 +1971,16 @@
         <v>13</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1994,16 +1994,16 @@
         <v>13</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -2017,16 +2017,16 @@
         <v>13</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2040,16 +2040,16 @@
         <v>13</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2063,16 +2063,16 @@
         <v>13</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -2086,16 +2086,16 @@
         <v>13</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -2109,16 +2109,16 @@
         <v>18</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="2:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2131,17 +2131,17 @@
       <c r="D38" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>153</v>
+      <c r="G38" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>150</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
@@ -2155,19 +2155,19 @@
         <v>18</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>89</v>
       </c>
@@ -2178,19 +2178,19 @@
         <v>13</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="J40" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H40" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="K40" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2203,23 +2203,23 @@
       <c r="D41" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="21" t="s">
-        <v>199</v>
+      <c r="F41" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>93</v>
       </c>
@@ -2230,19 +2230,19 @@
         <v>13</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H42" s="28" t="s">
-        <v>172</v>
+        <v>145</v>
+      </c>
+      <c r="H42" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
@@ -2256,20 +2256,20 @@
         <v>18</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -2283,16 +2283,16 @@
         <v>13</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -2306,16 +2306,16 @@
         <v>18</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -2329,16 +2329,16 @@
         <v>13</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
@@ -2352,16 +2352,16 @@
         <v>18</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2376,45 +2376,41 @@
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>177</v>
-      </c>
+      <c r="F49" s="8"/>
       <c r="G49" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I49" s="22" t="s">
-        <v>179</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I49" s="22"/>
       <c r="J49" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="2:11" ht="60" x14ac:dyDescent="0.25">
@@ -2428,22 +2424,22 @@
         <v>13</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
@@ -2457,52 +2453,49 @@
         <v>18</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="K52" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>115</v>
       </c>
@@ -2512,23 +2505,19 @@
       <c r="D53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="6" t="s">
-        <v>185</v>
-      </c>
+      <c r="F53" s="6"/>
       <c r="G53" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I53" s="22" t="s">
-        <v>179</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I53" s="22"/>
       <c r="J53" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -2542,20 +2531,20 @@
         <v>13</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2566,167 +2555,176 @@
         <v>120</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>188</v>
+        <v>176</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" t="s">
         <v>122</v>
-      </c>
-      <c r="C56" t="s">
-        <v>123</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="I56" s="24" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" t="s">
         <v>124</v>
       </c>
-      <c r="C57" t="s">
-        <v>125</v>
-      </c>
       <c r="D57" t="s">
         <v>13</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" t="s">
         <v>128</v>
       </c>
-      <c r="C59" t="s">
-        <v>129</v>
-      </c>
       <c r="D59" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" t="s">
         <v>130</v>
       </c>
-      <c r="C60" t="s">
-        <v>131</v>
-      </c>
       <c r="D60" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" t="s">
         <v>132</v>
-      </c>
-      <c r="C61" t="s">
-        <v>133</v>
       </c>
       <c r="D61" t="s">
         <v>18</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CARLA-3 Corrected DPEs and DD
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B372665-AF15-4E85-9FDC-57F97ABD663F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB19027-8E92-427B-B893-880C8A5872DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="191">
   <si>
     <t>index</t>
   </si>
@@ -499,30 +499,18 @@
     <t>diabetes2</t>
   </si>
   <si>
-    <t>recode(1= 1; 2 = 0;)</t>
-  </si>
-  <si>
     <t>cvd</t>
   </si>
   <si>
-    <t>recode(0= 0; 1 = 1; 2=1;)</t>
-  </si>
-  <si>
     <t>cancer</t>
   </si>
   <si>
     <t>fam_diab</t>
   </si>
   <si>
-    <t>recode(1= 1; 2 = 0; 3=2; 8=2;)</t>
-  </si>
-  <si>
     <t>fam_cancer</t>
   </si>
   <si>
-    <t>f1_stroke_first_year_inc</t>
-  </si>
-  <si>
     <t>date of diagnose and the date of birth</t>
   </si>
   <si>
@@ -532,83 +520,103 @@
     <t>measured HF via echocardiography, symptoms and pBNP at FU1</t>
   </si>
   <si>
-    <t>f2_cancer1_inc</t>
-  </si>
-  <si>
-    <t>f2_cancer1_typ</t>
-  </si>
-  <si>
-    <t>f2_cancer1_date</t>
-  </si>
-  <si>
     <t>vit_stat</t>
   </si>
   <si>
-    <t>tod_dat</t>
-  </si>
-  <si>
-    <t>hyp_i</t>
-  </si>
-  <si>
     <t>fam_stroke</t>
   </si>
   <si>
-    <t>cignr_day</t>
-  </si>
-  <si>
-    <t>cignr_day*1</t>
-  </si>
-  <si>
-    <t>Amount of tobacco smoked currently per day, at time of diet assessment (conversion into grams: 1 cigarette = 1 gram of tobacco)</t>
-  </si>
-  <si>
     <t>recode(1= 1; 2 = 0; 9=0;)</t>
   </si>
   <si>
-    <t>birth_place</t>
+    <t>children</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>school;occup_edu;occup_edu_2; occup_edu_h; educ; educ3</t>
   </si>
   <si>
     <t>case_when(
-work_status == 1 ~ 0,                                                                                                    work_status == 2~ 1,                                                                                                       work_status == 3~ 5,                                                                                                             work_status == 4 ~ 6;
+work_status == 1 ~ 0,                                                                                                                                work_status == 2~ 1,                                                                                                                                 work_status == 3~ 5,                                                                                                                                  work_status == 4 ~ 6,
 work_status== 5 | work_status == 6 ~ 7,
-work_status == 7 ~ 9,
-employ== 1 ~ 1,                                                                                                                            employ == 2 ~ 2,                                                                                                                              employ == 3 ~ 2,                                                                                                                    employ== 4 ~ 7, TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> f2_mi_i_inc</t>
-  </si>
-  <si>
-    <t>f2_mi_year</t>
-  </si>
-  <si>
-    <t>f2_stoke_i_inc</t>
-  </si>
-  <si>
-    <t>f1_age</t>
-  </si>
-  <si>
-    <t>children</t>
-  </si>
-  <si>
-    <t>undetermined</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>school;occup_edu;occup_edu_2; occup_edu_h; educ; educ3</t>
+work_status == 9 ~ 7,
+employ== 1 ~ 1,                                                                                                                                                   employ == 2 ~ 2,                                                                                                                                                     employ == 3 ~ 2,                                                                                                                                              employ== 4 ~ 7, TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>cignr_day;cigarnr_day;pipe_day;tabacconr_day</t>
+  </si>
+  <si>
+    <t>__BLANK__</t>
+  </si>
+  <si>
+    <t>paste</t>
+  </si>
+  <si>
+    <t>case_when(                                                                                                                                                                                                                                                                                                                                                                                                                                !is.na(hyp_i) &amp; hyp_i == 1 ~ 1,                                                                                                                                                   !is.na(hyp_i) &amp; hyp_i == 2 ~ 0,                                                                                is.na(hyp_i) &amp; htn_kora == 1 ~ 1,                                                            is.na(hyp_i) &amp; htn_kora == 0 ~ 0,  TRUE ~ NA_real_  )</t>
+  </si>
+  <si>
+    <t>hyp_i; htn_kora</t>
+  </si>
+  <si>
+    <t>recode(0= 0; 1 = 1; 2=0;)</t>
+  </si>
+  <si>
+    <t>recode(1= 1; 2 = 0; 3=0; 8=2;)</t>
+  </si>
+  <si>
+    <t>f1_htn_kora ;f2_htn_kora</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>tod_dat;gebdat</t>
+  </si>
+  <si>
+    <t>f2_insuff_date;gebdat</t>
+  </si>
+  <si>
+    <t>tod_dat-gebdat</t>
+  </si>
+  <si>
+    <t>f2_insuff_date-gebdat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> case_when(
+fr_op7 == 2 ~ 3, 
+fr_period1 == 3 &amp; age &gt;= 45 ~ 1,
+fr_period1 == 2 &amp; age &gt;= 45 &amp; age &lt;= 55 ~ 2,
+ fr_period1 %in% c(1, 2) &amp; age &lt; 45 ~ 0,
+ fr_period1 == 3 &amp; age &lt; 45 ~ 0,
+  TRUE ~ NA_real_
+    )</t>
+  </si>
+  <si>
+    <t>fr_period1;fr_op7</t>
   </si>
   <si>
     <t>case_when(
-school %in% c(5,6)|occup_edu%in% c(7)|occup_edu_2  %in% c(7)|occup_edu_h%in% c(7)|educ %in% c(7)~ 7,                                                                                                                                               school%in% c(5,6)|occup_edu %in% c(6)|occup_edu_2  %in% c(6)|occup_edu_h%in% c(6)|educ%in% c(6)~ 6L,                                                                                                                                       school %in% c(5,6)|occup_edu%in% c(5)|occup_edu_2  %in% c(5)|occup_edu_h%in% c(5)|educ%in% c(5)~ 5L,                                                                                                                                 school %in% c(5,6)|occup_edu%in% c(4)|occup_edu_2 %in% c(4)|occup_edu_h%in% c(4)|educ%in% c(4)~ 4L,                                                                                                                         school %in% c(3,4)|occup_edu  %in% c(3)|occup_edu_2%in%c(3)|occup_edu_h%in% c(3)|educ %in% c(3)|educ3%in% c(3)~ 3L,                                                                                    school  %in% c(2)|occup_edu %in% c(2)|occup_edu_2 %in% c(2)|occup_edu_h%in% c(2)|educ %in% c(2)|educ3%in% c(2)~ 2L,                                                                                    school  %in% c(1)|occup_edu %in% c(1)|occup_edu_2 %in% c(1)|occup_edu_h%in% c(1)|educ %in% c(1)|educ3%in% c(1)~ 1L,                                       
+school %in% c(5,6)&amp;occup_edu%in% c(7)|occup_edu_2  %in% c(7)|occup_edu_h%in% c(7)|educ %in% c(7)~ 7,                                                                                                                                               school%in% c(5,6)&amp;occup_edu %in% c(6)|occup_edu_2  %in% c(6)|occup_edu_h%in% c(6)|educ%in% c(6)~ 6L,                                                                                                                                       school %in% c(5,6)|occup_edu%in% c(5)|occup_edu_2  %in% c(5)|occup_edu_h%in% c(5)|educ%in% c(5)~ 5L,                                                                                                                                 school %in% c(5,6)|occup_edu%in% c(4)|occup_edu_2 %in% c(4)|occup_edu_h%in% c(4)|educ%in% c(4)~ 3L,                                                                                                                         school %in% c(3,4)|occup_edu  %in% c(2,3)|occup_edu_2%in%c(2,3)|occup_edu_h%in% c(2,3)|educ %in% c(2,3)|educ3%in% c(2,3)~ 2L,                                                                                    school  %in% c(2)~ 2L,                                                                                                                                 school  %in% c(1)|occup_edu %in% c(1)|occup_edu_2 %in% c(1)|occup_edu_h%in% c(1)|educ %in% c(1)|educ3%in% c(1)~ 1L,                                       
 school  %in% c(7)|occup_edu%in% c(8)|occup_edu_2  %in% c(8)|occup_edu_h%in% c(8)~ 9L,                                                                                                                                                                 TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>cignr_day*1+cigarnr_day*5+pipe_day*5+tabacconr_day</t>
+  </si>
+  <si>
+    <t>case_when(
+      f1_htn_kora == 1 | f2_htn_kora == 1 ~ 1,
+      f1_htn_kora == 0 &amp; f2_htn_kora == 0 ~ 0,
+      TRUE ~ NA_real_
+    )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,13 +628,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,21 +646,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -693,79 +680,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1108,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,29 +1127,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="12" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1195,71 +1163,71 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="23" customFormat="1" ht="270" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="D5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="J5" s="12" t="s">
+      <c r="H5" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="13" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1273,19 +1241,19 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1299,70 +1267,72 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="23" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+    <row r="8" spans="1:11" s="12" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="21" t="s">
+      <c r="D8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="J8" s="12" t="s">
+      <c r="H8" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="H9" s="24"/>
-      <c r="J9" s="8" t="s">
+      <c r="D9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>149</v>
+      <c r="K9" s="12" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1375,16 +1345,16 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K10" s="5" t="s">
+      <c r="G10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1398,23 +1368,23 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1424,22 +1394,20 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="H12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1453,19 +1421,19 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1479,80 +1447,82 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:11" s="12" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>150</v>
+      <c r="D15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>186</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="21" t="s">
+      <c r="D16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H16" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="J16" s="12" t="s">
+      <c r="H16" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="8" t="s">
@@ -1578,19 +1548,19 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="F18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1604,16 +1574,16 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K19" s="5" t="s">
+      <c r="G19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1627,41 +1597,39 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="2:11" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>175</v>
+      <c r="D21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>159</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="H21" s="9"/>
       <c r="J21" s="8" t="s">
         <v>148</v>
       </c>
@@ -1669,30 +1637,29 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="G22" s="14" t="s">
+      <c r="D22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16" t="s">
+      <c r="H22" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="K22" s="8" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1706,46 +1673,46 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G23" s="4" t="s">
+      <c r="F23" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+    <row r="24" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="D24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>140</v>
+      <c r="H24" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1758,20 +1725,20 @@
       <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>163</v>
+      <c r="F25" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="G25" t="s">
         <v>145</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>140</v>
+      <c r="H25" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1784,20 +1751,20 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>165</v>
+      <c r="F26" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="G26" t="s">
         <v>145</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>140</v>
+      <c r="H26" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1810,16 +1777,16 @@
       <c r="D27" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K27" s="5" t="s">
+      <c r="G27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1833,16 +1800,16 @@
       <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K28" s="5" t="s">
+      <c r="G28" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1856,16 +1823,16 @@
       <c r="D29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K29" s="5" t="s">
+      <c r="G29" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1879,16 +1846,16 @@
       <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K30" s="5" t="s">
+      <c r="G30" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1902,16 +1869,16 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K31" s="5" t="s">
+      <c r="G31" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1925,16 +1892,16 @@
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K32" s="5" t="s">
+      <c r="G32" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1948,63 +1915,69 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K33" s="5" t="s">
+      <c r="G33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+    <row r="34" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="D34" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>188</v>
+      <c r="D35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -2017,16 +1990,16 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="K36" s="18" t="s">
+      <c r="G36" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="K36" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2040,39 +2013,39 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K37" s="5" t="s">
+      <c r="G37" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="2:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
+    <row r="38" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="K38" s="12" t="s">
+      <c r="D38" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K38" s="8" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2086,122 +2059,113 @@
       <c r="D39" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K39" s="5" t="s">
+      <c r="G39" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+    <row r="40" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+      <c r="D40" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
+      <c r="D41" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="D42" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>188</v>
+      <c r="F43" s="8"/>
+      <c r="G43" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -2214,16 +2178,16 @@
       <c r="D44" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K44" s="4" t="s">
+      <c r="G44" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K44" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2237,16 +2201,16 @@
       <c r="D45" t="s">
         <v>18</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K45" s="4" t="s">
+      <c r="G45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2260,16 +2224,16 @@
       <c r="D46" t="s">
         <v>13</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K46" s="4" t="s">
+      <c r="G46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2283,173 +2247,177 @@
       <c r="D47" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K47" s="4" t="s">
+      <c r="G47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K47" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
+    <row r="48" spans="2:11" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
+      <c r="D48" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I49" s="20"/>
-      <c r="J49" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="D49" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="D50" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" s="12" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I51" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I53" s="20"/>
-      <c r="J53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>188</v>
+      <c r="F53" s="11"/>
+      <c r="G53" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I53" s="16"/>
+      <c r="J53" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -2462,129 +2430,120 @@
       <c r="D54" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
+      <c r="F54" s="11"/>
+      <c r="G54" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="D55" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K55" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="F56" s="11"/>
+      <c r="G56" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I56" s="16"/>
+      <c r="J56" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D57" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
+      <c r="D57" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K57" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F58" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>188</v>
+      <c r="F58" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -2597,17 +2556,17 @@
       <c r="D59" t="s">
         <v>13</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K59" s="4" t="s">
+      <c r="G59" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K59" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2621,17 +2580,17 @@
       <c r="D60" t="s">
         <v>13</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K60" s="4" t="s">
+      <c r="G60" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K60" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2645,17 +2604,17 @@
       <c r="D61" t="s">
         <v>18</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K61" s="4" t="s">
+      <c r="G61" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K61" s="3" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CARLA-3 DPEs and DD of covariate,chronic diseases
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB19027-8E92-427B-B893-880C8A5872DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C90B59-5358-4D93-B3A4-955EBC68F5F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,9 +535,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>school;occup_edu;occup_edu_2; occup_edu_h; educ; educ3</t>
-  </si>
-  <si>
     <t>case_when(
 work_status == 1 ~ 0,                                                                                                                                work_status == 2~ 1,                                                                                                                                 work_status == 3~ 5,                                                                                                                                  work_status == 4 ~ 6,
 work_status== 5 | work_status == 6 ~ 7,
@@ -597,11 +594,6 @@
     <t>fr_period1;fr_op7</t>
   </si>
   <si>
-    <t>case_when(
-school %in% c(5,6)&amp;occup_edu%in% c(7)|occup_edu_2  %in% c(7)|occup_edu_h%in% c(7)|educ %in% c(7)~ 7,                                                                                                                                               school%in% c(5,6)&amp;occup_edu %in% c(6)|occup_edu_2  %in% c(6)|occup_edu_h%in% c(6)|educ%in% c(6)~ 6L,                                                                                                                                       school %in% c(5,6)|occup_edu%in% c(5)|occup_edu_2  %in% c(5)|occup_edu_h%in% c(5)|educ%in% c(5)~ 5L,                                                                                                                                 school %in% c(5,6)|occup_edu%in% c(4)|occup_edu_2 %in% c(4)|occup_edu_h%in% c(4)|educ%in% c(4)~ 3L,                                                                                                                         school %in% c(3,4)|occup_edu  %in% c(2,3)|occup_edu_2%in%c(2,3)|occup_edu_h%in% c(2,3)|educ %in% c(2,3)|educ3%in% c(2,3)~ 2L,                                                                                    school  %in% c(2)~ 2L,                                                                                                                                 school  %in% c(1)|occup_edu %in% c(1)|occup_edu_2 %in% c(1)|occup_edu_h%in% c(1)|educ %in% c(1)|educ3%in% c(1)~ 1L,                                       
-school  %in% c(7)|occup_edu%in% c(8)|occup_edu_2  %in% c(8)|occup_edu_h%in% c(8)~ 9L,                                                                                                                                                                 TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>cignr_day*1+cigarnr_day*5+pipe_day*5+tabacconr_day</t>
   </si>
   <si>
@@ -610,6 +602,14 @@
       f1_htn_kora == 0 &amp; f2_htn_kora == 0 ~ 0,
       TRUE ~ NA_real_
     )</t>
+  </si>
+  <si>
+    <t>school;occup_edu_h</t>
+  </si>
+  <si>
+    <t>case_when(
+school %in% c(5,6)&amp;occup_edu_h%in% c(7)~ 7,                                                                                                                                               school%in% c(5,6)&amp;occup_edu_h%in% c(6)~ 6L,                                                                                                                                       school %in% c(5,6)|occup_edu_h%in% c(5)~ 5L,                                                                                                                                 school %in% c(3,4)|occup_edu_h%in% c(4)~ 4L,                                                                                                                         school %in% c(3,4)|occup_edu_h%in% c(3)~ 4L,                                                                                                                                 school  %in% c(1)|occup_edu_h%in% c(1)~ 1L,                                       
+school  %in% c(7)|occup_edu_h%in% c(8)~ 9L,                                                                                                                                                                 TRUE ~ NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1205,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>19</v>
       </c>
@@ -1216,13 +1216,13 @@
         <v>13</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>139</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>134</v>
@@ -1300,7 +1300,7 @@
         <v>139</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>134</v>
@@ -1320,10 +1320,10 @@
         <v>13</v>
       </c>
       <c r="F9" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>174</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>175</v>
       </c>
       <c r="H9" s="15">
         <v>0</v>
@@ -1395,13 +1395,13 @@
         <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="4" t="s">
@@ -1474,13 +1474,13 @@
         <v>13</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>139</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>134</v>
@@ -1624,10 +1624,10 @@
         <v>13</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H21" s="9"/>
       <c r="J21" s="8" t="s">
@@ -1654,7 +1654,7 @@
         <v>145</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>148</v>
@@ -1706,7 +1706,7 @@
         <v>145</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>148</v>
@@ -1732,7 +1732,7 @@
         <v>145</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>148</v>
@@ -1758,7 +1758,7 @@
         <v>145</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>148</v>
@@ -2271,13 +2271,13 @@
         <v>13</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>139</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J48" s="12" t="s">
         <v>134</v>
@@ -2294,7 +2294,7 @@
         <v>108</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>107</v>
@@ -2353,13 +2353,13 @@
         <v>170</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>142</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I51" s="16" t="s">
         <v>163</v>
@@ -2531,13 +2531,13 @@
         <v>18</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G58" s="12" t="s">
         <v>142</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J58" s="12" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
finalising DD and DPEs for CARLA
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_CARLA_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65878836-7FAD-4121-8313-AC55795CBCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DB094F-74D0-4B7C-955D-9E9AC5039E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="203">
   <si>
     <t>index</t>
   </si>
@@ -621,12 +621,6 @@
     <t>f1_htn_kora;f2_htn_kora;f1_untdat;f2_untdat;gebdat</t>
   </si>
   <si>
-    <t>(tod_dat-gebdat)/365.25</t>
-  </si>
-  <si>
-    <t>(f2_insuff_date-gebdat)/365.25</t>
-  </si>
-  <si>
     <t>case_when(
       f1_htn_kora == 1 | f2_htn_kora == 1 ~ 1,
       f1_htn_kora == 0 &amp; f2_htn_kora == 0 ~ 0,
@@ -676,6 +670,19 @@
   f2_htn_kora == 1 ~ as.numeric(f2_untdat - gebdat)/365.25,  
   TRUE ~ NA_real_
 )</t>
+  </si>
+  <si>
+    <t>as.numeric(pmax(((f1_untdat - gebdat)/365.25),
+                ((f2_untdat - gebdat)/365.25),na.rm = TRUE))</t>
+  </si>
+  <si>
+    <t>gebdat;f1_untdat;f2_untdat</t>
+  </si>
+  <si>
+    <t>as.numeric(f2_insuff_date-gebdat)/365.25</t>
+  </si>
+  <si>
+    <t>as.numeric(tod_dat-gebdat)/365.25</t>
   </si>
 </sst>
 </file>
@@ -746,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -805,6 +812,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1112,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1447,7 @@
         <v>142</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="4" t="s">
@@ -1516,10 +1526,10 @@
         <v>139</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>134</v>
@@ -1669,7 +1679,7 @@
         <v>139</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>147</v>
@@ -1747,10 +1757,10 @@
         <v>145</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>147</v>
@@ -1776,10 +1786,10 @@
         <v>145</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>147</v>
@@ -1805,10 +1815,10 @@
         <v>145</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>147</v>
@@ -2333,7 +2343,7 @@
         <v>139</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>182</v>
@@ -2362,7 +2372,7 @@
         <v>139</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I49" s="14" t="s">
         <v>183</v>
@@ -2420,7 +2430,7 @@
         <v>142</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="I51" s="16" t="s">
         <v>162</v>
@@ -2598,7 +2608,7 @@
         <v>142</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="I58" s="14" t="s">
         <v>181</v>
@@ -2658,7 +2668,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>131</v>
       </c>
@@ -2668,18 +2678,21 @@
       <c r="D61" t="s">
         <v>18</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>149</v>
+      <c r="F61" t="s">
+        <v>200</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>199</v>
       </c>
       <c r="I61" s="3"/>
-      <c r="J61" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>150</v>
+      <c r="J61" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>